<commit_message>
Updating worksheet name in sample worksheet
</commit_message>
<xml_diff>
--- a/t/media_example.xlsx
+++ b/t/media_example.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Media" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="media_example" localSheetId="0">Sheet1!$A$1:$D$23</definedName>
+    <definedName name="media_example" localSheetId="0">Media!$A$1:$D$23</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="media_example.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:seaver:Software:KBase_Repos:transform:t:media_example.txt">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:seaver:Software:KBase_Repos:transform:t:media_example.txt">
       <textFields>
         <textField/>
       </textFields>

</xml_diff>